<commit_message>
Implement trust-based isolation and BCA data import
</commit_message>
<xml_diff>
--- a/DATA FOR IMPORT EXPORT/Template for Bulk Student Import.xlsx
+++ b/DATA FOR IMPORT EXPORT/Template for Bulk Student Import.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\CMSv5\DATA FOR IMPORT EXPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E876826-47DC-4214-82A0-309643F8A636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008CE8C3-6869-4303-AE85-5B14101B1D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sem-3" sheetId="1" r:id="rId1"/>
+    <sheet name="Sem2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -486,46 +486,46 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.44140625" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="33.44140625" customWidth="1"/>
-    <col min="32" max="32" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="33.42578125" customWidth="1"/>
+    <col min="32" max="32" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="32" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,417 +632,417 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O2" s="1"/>
       <c r="V2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O3" s="1"/>
       <c r="V3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O4" s="1"/>
       <c r="V4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O5" s="3"/>
       <c r="V5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O6" s="3"/>
       <c r="V6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O7" s="3"/>
       <c r="V7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O8" s="3"/>
       <c r="V8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O9" s="3"/>
       <c r="V9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O10" s="1"/>
       <c r="V10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O11" s="3"/>
       <c r="V11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O12" s="1"/>
       <c r="V12" s="1"/>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O13" s="1"/>
       <c r="V13" s="1"/>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O14" s="1"/>
       <c r="V14" s="1"/>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O15" s="1"/>
       <c r="V15" s="1"/>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O16" s="1"/>
       <c r="V16" s="1"/>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O17" s="3"/>
       <c r="V17" s="1"/>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O18" s="1"/>
       <c r="V18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O19" s="3"/>
       <c r="V19" s="1"/>
       <c r="AI19" s="1"/>
     </row>
-    <row r="20" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O20" s="3"/>
       <c r="V20" s="1"/>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O21" s="1"/>
       <c r="V21" s="1"/>
       <c r="AI21" s="1"/>
     </row>
-    <row r="22" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O22" s="3"/>
       <c r="V22" s="1"/>
       <c r="AI22" s="1"/>
     </row>
-    <row r="23" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O23" s="1"/>
       <c r="V23" s="1"/>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O24" s="1"/>
       <c r="V24" s="1"/>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O25" s="3"/>
       <c r="V25" s="1"/>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O26" s="1"/>
       <c r="V26" s="1"/>
       <c r="AI26" s="1"/>
     </row>
-    <row r="27" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O27" s="1"/>
       <c r="V27" s="1"/>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O28" s="1"/>
       <c r="V28" s="1"/>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O29" s="1"/>
       <c r="V29" s="1"/>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O30" s="3"/>
       <c r="V30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O31" s="3"/>
       <c r="V31" s="1"/>
       <c r="AI31" s="1"/>
     </row>
-    <row r="32" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O32" s="1"/>
       <c r="V32" s="1"/>
       <c r="AI32" s="1"/>
     </row>
-    <row r="33" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O33" s="3"/>
       <c r="V33" s="1"/>
       <c r="AI33" s="1"/>
     </row>
-    <row r="34" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O34" s="3"/>
       <c r="V34" s="1"/>
       <c r="AI34" s="1"/>
     </row>
-    <row r="35" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O35" s="1"/>
       <c r="V35" s="1"/>
       <c r="AI35" s="1"/>
     </row>
-    <row r="36" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O36" s="1"/>
       <c r="V36" s="1"/>
       <c r="AI36" s="1"/>
     </row>
-    <row r="37" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O37" s="3"/>
       <c r="V37" s="1"/>
       <c r="AI37" s="1"/>
     </row>
-    <row r="38" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O38" s="1"/>
       <c r="V38" s="1"/>
       <c r="AI38" s="1"/>
     </row>
-    <row r="39" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O39" s="3"/>
       <c r="V39" s="1"/>
       <c r="AI39" s="1"/>
     </row>
-    <row r="40" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O40" s="3"/>
       <c r="V40" s="1"/>
       <c r="AI40" s="1"/>
     </row>
-    <row r="41" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O41" s="1"/>
       <c r="V41" s="1"/>
       <c r="AI41" s="1"/>
     </row>
-    <row r="42" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O42" s="3"/>
       <c r="V42" s="1"/>
       <c r="AI42" s="1"/>
     </row>
-    <row r="43" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O43" s="1"/>
       <c r="V43" s="1"/>
       <c r="AI43" s="1"/>
     </row>
-    <row r="44" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O44" s="1"/>
       <c r="V44" s="1"/>
       <c r="AI44" s="1"/>
     </row>
-    <row r="45" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O45" s="1"/>
       <c r="V45" s="1"/>
       <c r="AI45" s="1"/>
     </row>
-    <row r="46" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O46" s="1"/>
       <c r="V46" s="1"/>
       <c r="AI46" s="1"/>
     </row>
-    <row r="47" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O47" s="1"/>
       <c r="V47" s="1"/>
       <c r="AI47" s="1"/>
     </row>
-    <row r="48" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O48" s="3"/>
       <c r="V48" s="1"/>
       <c r="AI48" s="1"/>
     </row>
-    <row r="49" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O49" s="1"/>
       <c r="V49" s="1"/>
       <c r="AI49" s="1"/>
     </row>
-    <row r="50" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O50" s="1"/>
       <c r="V50" s="1"/>
       <c r="AI50" s="1"/>
     </row>
-    <row r="51" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O51" s="1"/>
       <c r="V51" s="1"/>
       <c r="AI51" s="1"/>
     </row>
-    <row r="52" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O52" s="1"/>
       <c r="V52" s="1"/>
       <c r="AI52" s="1"/>
     </row>
-    <row r="53" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O53" s="1"/>
       <c r="V53" s="1"/>
       <c r="AI53" s="1"/>
     </row>
-    <row r="54" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O54" s="3"/>
       <c r="V54" s="1"/>
       <c r="AI54" s="1"/>
     </row>
-    <row r="55" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O55" s="1"/>
       <c r="V55" s="1"/>
       <c r="AI55" s="1"/>
     </row>
-    <row r="56" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O56" s="1"/>
       <c r="V56" s="1"/>
       <c r="AI56" s="1"/>
     </row>
-    <row r="57" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O57" s="3"/>
       <c r="V57" s="1"/>
       <c r="AI57" s="1"/>
     </row>
-    <row r="58" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O58" s="3"/>
       <c r="V58" s="1"/>
       <c r="AI58" s="1"/>
     </row>
-    <row r="59" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O59" s="1"/>
       <c r="V59" s="1"/>
       <c r="AI59" s="1"/>
     </row>
-    <row r="60" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O60" s="1"/>
       <c r="V60" s="1"/>
       <c r="AI60" s="1"/>
     </row>
-    <row r="61" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O61" s="1"/>
       <c r="V61" s="1"/>
       <c r="AI61" s="1"/>
     </row>
-    <row r="62" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O62" s="3"/>
       <c r="V62" s="1"/>
       <c r="AI62" s="1"/>
     </row>
-    <row r="63" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O63" s="1"/>
       <c r="V63" s="1"/>
       <c r="AI63" s="1"/>
     </row>
-    <row r="64" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O64" s="3"/>
       <c r="V64" s="1"/>
       <c r="AI64" s="1"/>
     </row>
-    <row r="65" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O65" s="1"/>
       <c r="V65" s="1"/>
       <c r="AI65" s="1"/>
     </row>
-    <row r="66" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O66" s="1"/>
       <c r="V66" s="1"/>
       <c r="AI66" s="1"/>
     </row>
-    <row r="67" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O67" s="3"/>
       <c r="V67" s="1"/>
       <c r="AI67" s="1"/>
     </row>
-    <row r="68" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O68" s="3"/>
       <c r="V68" s="1"/>
       <c r="AI68" s="1"/>
     </row>
-    <row r="69" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O69" s="1"/>
       <c r="V69" s="1"/>
       <c r="AI69" s="1"/>
     </row>
-    <row r="70" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O70" s="1"/>
       <c r="V70" s="1"/>
       <c r="AI70" s="1"/>
     </row>
-    <row r="71" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O71" s="3"/>
       <c r="V71" s="1"/>
       <c r="AI71" s="1"/>
     </row>
-    <row r="72" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O72" s="1"/>
       <c r="V72" s="1"/>
       <c r="AI72" s="1"/>
     </row>
-    <row r="73" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O73" s="1"/>
       <c r="V73" s="1"/>
       <c r="AI73" s="1"/>
     </row>
-    <row r="74" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O74" s="3"/>
       <c r="V74" s="1"/>
       <c r="AI74" s="1"/>
     </row>
-    <row r="75" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O75" s="3"/>
       <c r="V75" s="1"/>
       <c r="AI75" s="1"/>
     </row>
-    <row r="76" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O76" s="1"/>
       <c r="V76" s="1"/>
       <c r="AI76" s="1"/>
     </row>
-    <row r="77" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O77" s="1"/>
       <c r="V77" s="1"/>
       <c r="AI77" s="1"/>
     </row>
-    <row r="78" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O78" s="1"/>
       <c r="V78" s="1"/>
       <c r="AI78" s="1"/>
     </row>
-    <row r="79" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O79" s="3"/>
       <c r="V79" s="1"/>
       <c r="AI79" s="1"/>
     </row>
-    <row r="80" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O80" s="3"/>
       <c r="V80" s="1"/>
       <c r="AI80" s="1"/>
     </row>
-    <row r="81" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O81" s="3"/>
       <c r="V81" s="1"/>
       <c r="AI81" s="1"/>
     </row>
-    <row r="82" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O82" s="3"/>
       <c r="V82" s="1"/>
       <c r="AI82" s="1"/>
     </row>
-    <row r="83" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O83" s="3"/>
       <c r="V83" s="1"/>
       <c r="AI83" s="1"/>
     </row>
-    <row r="84" spans="15:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="15:35" x14ac:dyDescent="0.25">
       <c r="O84" s="1"/>
       <c r="V84" s="1"/>
       <c r="AI84" s="1"/>
@@ -1058,7 +1058,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>